<commit_message>
Includes Team_Name into Data
</commit_message>
<xml_diff>
--- a/Player_Stats_Per_Map.xlsx
+++ b/Player_Stats_Per_Map.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M121"/>
+  <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,11 @@
           <t>+/–.1</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -546,6 +551,11 @@
       <c r="M2" t="n">
         <v>1</v>
       </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -593,6 +603,11 @@
       <c r="M3" t="n">
         <v>-1</v>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -640,6 +655,11 @@
       <c r="M4" t="n">
         <v>2</v>
       </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -687,6 +707,11 @@
       <c r="M5" t="n">
         <v>0</v>
       </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -734,6 +759,11 @@
       <c r="M6" t="n">
         <v>-2</v>
       </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -781,6 +811,11 @@
       <c r="M7" t="n">
         <v>5</v>
       </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -828,6 +863,11 @@
       <c r="M8" t="n">
         <v>0</v>
       </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -875,6 +915,11 @@
       <c r="M9" t="n">
         <v>-2</v>
       </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -922,6 +967,11 @@
       <c r="M10" t="n">
         <v>-1</v>
       </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -969,6 +1019,11 @@
       <c r="M11" t="n">
         <v>-2</v>
       </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1016,6 +1071,11 @@
       <c r="M12" t="n">
         <v>2</v>
       </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1063,6 +1123,11 @@
       <c r="M13" t="n">
         <v>1</v>
       </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1110,6 +1175,11 @@
       <c r="M14" t="n">
         <v>-2</v>
       </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1157,6 +1227,11 @@
       <c r="M15" t="n">
         <v>-2</v>
       </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1204,6 +1279,11 @@
       <c r="M16" t="n">
         <v>-2</v>
       </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>GEN</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1251,6 +1331,11 @@
       <c r="M17" t="n">
         <v>2</v>
       </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1298,6 +1383,11 @@
       <c r="M18" t="n">
         <v>-1</v>
       </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1345,6 +1435,11 @@
       <c r="M19" t="n">
         <v>1</v>
       </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1392,6 +1487,11 @@
       <c r="M20" t="n">
         <v>1</v>
       </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1439,6 +1539,11 @@
       <c r="M21" t="n">
         <v>0</v>
       </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>RRQ</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1486,6 +1591,11 @@
       <c r="M22" t="n">
         <v>4</v>
       </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1533,6 +1643,11 @@
       <c r="M23" t="n">
         <v>-1</v>
       </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1580,6 +1695,11 @@
       <c r="M24" t="n">
         <v>0</v>
       </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1627,6 +1747,11 @@
       <c r="M25" t="n">
         <v>-5</v>
       </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1674,6 +1799,11 @@
       <c r="M26" t="n">
         <v>-2</v>
       </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1721,6 +1851,11 @@
       <c r="M27" t="n">
         <v>1</v>
       </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1768,6 +1903,11 @@
       <c r="M28" t="n">
         <v>5</v>
       </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1815,6 +1955,11 @@
       <c r="M29" t="n">
         <v>-1</v>
       </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1862,6 +2007,11 @@
       <c r="M30" t="n">
         <v>0</v>
       </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1909,6 +2059,11 @@
       <c r="M31" t="n">
         <v>-1</v>
       </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1956,6 +2111,11 @@
       <c r="M32" t="n">
         <v>3</v>
       </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2003,6 +2163,11 @@
       <c r="M33" t="n">
         <v>3</v>
       </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2050,6 +2215,11 @@
       <c r="M34" t="n">
         <v>0</v>
       </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2097,6 +2267,11 @@
       <c r="M35" t="n">
         <v>-1</v>
       </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2144,6 +2319,11 @@
       <c r="M36" t="n">
         <v>-2</v>
       </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2191,6 +2371,11 @@
       <c r="M37" t="n">
         <v>2</v>
       </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2238,6 +2423,11 @@
       <c r="M38" t="n">
         <v>1</v>
       </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2285,6 +2475,11 @@
       <c r="M39" t="n">
         <v>-2</v>
       </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2332,6 +2527,11 @@
       <c r="M40" t="n">
         <v>-1</v>
       </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2379,6 +2579,11 @@
       <c r="M41" t="n">
         <v>-3</v>
       </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2426,6 +2631,11 @@
       <c r="M42" t="n">
         <v>0</v>
       </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2473,6 +2683,11 @@
       <c r="M43" t="n">
         <v>0</v>
       </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2520,6 +2735,11 @@
       <c r="M44" t="n">
         <v>1</v>
       </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2567,6 +2787,11 @@
       <c r="M45" t="n">
         <v>1</v>
       </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2614,6 +2839,11 @@
       <c r="M46" t="n">
         <v>3</v>
       </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2661,6 +2891,11 @@
       <c r="M47" t="n">
         <v>-2</v>
       </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2708,6 +2943,11 @@
       <c r="M48" t="n">
         <v>-2</v>
       </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2755,6 +2995,11 @@
       <c r="M49" t="n">
         <v>-1</v>
       </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2802,6 +3047,11 @@
       <c r="M50" t="n">
         <v>1</v>
       </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2849,6 +3099,11 @@
       <c r="M51" t="n">
         <v>-1</v>
       </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2896,6 +3151,11 @@
       <c r="M52" t="n">
         <v>2</v>
       </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2943,6 +3203,11 @@
       <c r="M53" t="n">
         <v>-3</v>
       </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2990,6 +3255,11 @@
       <c r="M54" t="n">
         <v>1</v>
       </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3037,6 +3307,11 @@
       <c r="M55" t="n">
         <v>-3</v>
       </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3084,6 +3359,11 @@
       <c r="M56" t="n">
         <v>-1</v>
       </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3131,6 +3411,11 @@
       <c r="M57" t="n">
         <v>4</v>
       </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3178,6 +3463,11 @@
       <c r="M58" t="n">
         <v>2</v>
       </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3225,6 +3515,11 @@
       <c r="M59" t="n">
         <v>1</v>
       </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3272,6 +3567,11 @@
       <c r="M60" t="n">
         <v>0</v>
       </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3319,6 +3619,11 @@
       <c r="M61" t="n">
         <v>-3</v>
       </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3366,6 +3671,11 @@
       <c r="M62" t="n">
         <v>-1</v>
       </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3413,6 +3723,11 @@
       <c r="M63" t="n">
         <v>1</v>
       </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3460,6 +3775,11 @@
       <c r="M64" t="n">
         <v>-1</v>
       </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3507,6 +3827,11 @@
       <c r="M65" t="n">
         <v>0</v>
       </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3554,6 +3879,11 @@
       <c r="M66" t="n">
         <v>1</v>
       </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3601,6 +3931,11 @@
       <c r="M67" t="n">
         <v>-1</v>
       </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3648,6 +3983,11 @@
       <c r="M68" t="n">
         <v>0</v>
       </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3695,6 +4035,11 @@
       <c r="M69" t="n">
         <v>2</v>
       </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3742,6 +4087,11 @@
       <c r="M70" t="n">
         <v>-1</v>
       </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3789,6 +4139,11 @@
       <c r="M71" t="n">
         <v>0</v>
       </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3836,6 +4191,11 @@
       <c r="M72" t="n">
         <v>2</v>
       </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3883,6 +4243,11 @@
       <c r="M73" t="n">
         <v>-2</v>
       </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3930,6 +4295,11 @@
       <c r="M74" t="n">
         <v>1</v>
       </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3977,6 +4347,11 @@
       <c r="M75" t="n">
         <v>1</v>
       </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4024,6 +4399,11 @@
       <c r="M76" t="n">
         <v>-1</v>
       </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>BLD</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4071,6 +4451,11 @@
       <c r="M77" t="n">
         <v>2</v>
       </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4118,6 +4503,11 @@
       <c r="M78" t="n">
         <v>0</v>
       </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4165,6 +4555,11 @@
       <c r="M79" t="n">
         <v>-2</v>
       </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4212,6 +4607,11 @@
       <c r="M80" t="n">
         <v>0</v>
       </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4259,6 +4659,11 @@
       <c r="M81" t="n">
         <v>-1</v>
       </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4306,6 +4711,11 @@
       <c r="M82" t="n">
         <v>0</v>
       </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4353,6 +4763,11 @@
       <c r="M83" t="n">
         <v>-1</v>
       </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4400,6 +4815,11 @@
       <c r="M84" t="n">
         <v>1</v>
       </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4447,6 +4867,11 @@
       <c r="M85" t="n">
         <v>1</v>
       </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4494,6 +4919,11 @@
       <c r="M86" t="n">
         <v>-3</v>
       </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4541,6 +4971,11 @@
       <c r="M87" t="n">
         <v>-1</v>
       </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4588,6 +5023,11 @@
       <c r="M88" t="n">
         <v>7</v>
       </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4635,6 +5075,11 @@
       <c r="M89" t="n">
         <v>1</v>
       </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4682,6 +5127,11 @@
       <c r="M90" t="n">
         <v>-2</v>
       </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4729,6 +5179,11 @@
       <c r="M91" t="n">
         <v>-3</v>
       </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4776,6 +5231,11 @@
       <c r="M92" t="n">
         <v>6</v>
       </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4823,6 +5283,11 @@
       <c r="M93" t="n">
         <v>3</v>
       </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4870,6 +5335,11 @@
       <c r="M94" t="n">
         <v>1</v>
       </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4917,6 +5387,11 @@
       <c r="M95" t="n">
         <v>1</v>
       </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4964,6 +5439,11 @@
       <c r="M96" t="n">
         <v>0</v>
       </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5011,6 +5491,11 @@
       <c r="M97" t="n">
         <v>-3</v>
       </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5058,6 +5543,11 @@
       <c r="M98" t="n">
         <v>0</v>
       </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5105,6 +5595,11 @@
       <c r="M99" t="n">
         <v>-2</v>
       </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5152,6 +5647,11 @@
       <c r="M100" t="n">
         <v>-3</v>
       </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -5199,6 +5699,11 @@
       <c r="M101" t="n">
         <v>-3</v>
       </c>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -5246,6 +5751,11 @@
       <c r="M102" t="n">
         <v>5</v>
       </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5293,6 +5803,11 @@
       <c r="M103" t="n">
         <v>1</v>
       </c>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -5340,6 +5855,11 @@
       <c r="M104" t="n">
         <v>0</v>
       </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -5387,6 +5907,11 @@
       <c r="M105" t="n">
         <v>0</v>
       </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -5434,6 +5959,11 @@
       <c r="M106" t="n">
         <v>-3</v>
       </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -5481,6 +6011,11 @@
       <c r="M107" t="n">
         <v>1</v>
       </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5528,6 +6063,11 @@
       <c r="M108" t="n">
         <v>0</v>
       </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5575,6 +6115,11 @@
       <c r="M109" t="n">
         <v>-1</v>
       </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -5622,6 +6167,11 @@
       <c r="M110" t="n">
         <v>-1</v>
       </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5669,6 +6219,11 @@
       <c r="M111" t="n">
         <v>-2</v>
       </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -5716,6 +6271,11 @@
       <c r="M112" t="n">
         <v>1</v>
       </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5763,6 +6323,11 @@
       <c r="M113" t="n">
         <v>1</v>
       </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5810,6 +6375,11 @@
       <c r="M114" t="n">
         <v>5</v>
       </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5857,6 +6427,11 @@
       <c r="M115" t="n">
         <v>3</v>
       </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5904,6 +6479,11 @@
       <c r="M116" t="n">
         <v>0</v>
       </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>ZETA</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -5951,6 +6531,11 @@
       <c r="M117" t="n">
         <v>-4</v>
       </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5998,6 +6583,11 @@
       <c r="M118" t="n">
         <v>-2</v>
       </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -6045,6 +6635,11 @@
       <c r="M119" t="n">
         <v>-2</v>
       </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -6092,6 +6687,11 @@
       <c r="M120" t="n">
         <v>0</v>
       </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -6138,6 +6738,11 @@
       </c>
       <c r="M121" t="n">
         <v>-2</v>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted % to Decimal
</commit_message>
<xml_diff>
--- a/Player_Stats_Per_Map.xlsx
+++ b/Player_Stats_Per_Map.xlsx
@@ -529,18 +529,14 @@
       <c r="G2" t="n">
         <v>-10</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>45%</t>
-        </is>
+      <c r="H2" t="n">
+        <v>0.45</v>
       </c>
       <c r="I2" t="n">
         <v>55</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>17%</t>
-        </is>
+      <c r="J2" t="n">
+        <v>0.17</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -581,18 +577,14 @@
       <c r="G3" t="n">
         <v>-3</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>73%</t>
-        </is>
+      <c r="H3" t="n">
+        <v>0.73</v>
       </c>
       <c r="I3" t="n">
         <v>122</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>24%</t>
-        </is>
+      <c r="J3" t="n">
+        <v>0.24</v>
       </c>
       <c r="K3" t="n">
         <v>3</v>
@@ -633,18 +625,14 @@
       <c r="G4" t="n">
         <v>1</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H4" t="n">
+        <v>0.7</v>
       </c>
       <c r="I4" t="n">
         <v>120</v>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
+      <c r="J4" t="n">
+        <v>0.3</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -685,18 +673,14 @@
       <c r="G5" t="n">
         <v>-9</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>48%</t>
-        </is>
+      <c r="H5" t="n">
+        <v>0.48</v>
       </c>
       <c r="I5" t="n">
         <v>59</v>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>16%</t>
-        </is>
+      <c r="J5" t="n">
+        <v>0.16</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -737,18 +721,14 @@
       <c r="G6" t="n">
         <v>-2</v>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>61%</t>
-        </is>
+      <c r="H6" t="n">
+        <v>0.61</v>
       </c>
       <c r="I6" t="n">
         <v>112</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
+      <c r="J6" t="n">
+        <v>0.3</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -789,18 +769,14 @@
       <c r="G7" t="n">
         <v>-2</v>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>63%</t>
-        </is>
+      <c r="H7" t="n">
+        <v>0.63</v>
       </c>
       <c r="I7" t="n">
         <v>147</v>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J7" t="n">
+        <v>0.26</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -841,18 +817,14 @@
       <c r="G8" t="n">
         <v>-2</v>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>82%</t>
-        </is>
+      <c r="H8" t="n">
+        <v>0.82</v>
       </c>
       <c r="I8" t="n">
         <v>131</v>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>28%</t>
-        </is>
+      <c r="J8" t="n">
+        <v>0.28</v>
       </c>
       <c r="K8" t="n">
         <v>3</v>
@@ -893,18 +865,14 @@
       <c r="G9" t="n">
         <v>1</v>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>94%</t>
-        </is>
+      <c r="H9" t="n">
+        <v>0.9399999999999999</v>
       </c>
       <c r="I9" t="n">
         <v>125</v>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
+      <c r="J9" t="n">
+        <v>0.3</v>
       </c>
       <c r="K9" t="n">
         <v>1</v>
@@ -945,18 +913,14 @@
       <c r="G10" t="n">
         <v>10</v>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>79%</t>
-        </is>
+      <c r="H10" t="n">
+        <v>0.79</v>
       </c>
       <c r="I10" t="n">
         <v>187</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>20%</t>
-        </is>
+      <c r="J10" t="n">
+        <v>0.2</v>
       </c>
       <c r="K10" t="n">
         <v>3</v>
@@ -997,18 +961,14 @@
       <c r="G11" t="n">
         <v>-14</v>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>67%</t>
-        </is>
+      <c r="H11" t="n">
+        <v>0.67</v>
       </c>
       <c r="I11" t="n">
         <v>83</v>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>11%</t>
-        </is>
+      <c r="J11" t="n">
+        <v>0.11</v>
       </c>
       <c r="K11" t="n">
         <v>2</v>
@@ -1049,18 +1009,14 @@
       <c r="G12" t="n">
         <v>4</v>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
+      <c r="H12" t="n">
+        <v>0.75</v>
       </c>
       <c r="I12" t="n">
         <v>140</v>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>22%</t>
-        </is>
+      <c r="J12" t="n">
+        <v>0.22</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
@@ -1101,18 +1057,14 @@
       <c r="G13" t="n">
         <v>7</v>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>81%</t>
-        </is>
+      <c r="H13" t="n">
+        <v>0.8100000000000001</v>
       </c>
       <c r="I13" t="n">
         <v>216</v>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>18%</t>
-        </is>
+      <c r="J13" t="n">
+        <v>0.18</v>
       </c>
       <c r="K13" t="n">
         <v>6</v>
@@ -1153,18 +1105,14 @@
       <c r="G14" t="n">
         <v>6</v>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>71%</t>
-        </is>
+      <c r="H14" t="n">
+        <v>0.71</v>
       </c>
       <c r="I14" t="n">
         <v>155</v>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>37%</t>
-        </is>
+      <c r="J14" t="n">
+        <v>0.37</v>
       </c>
       <c r="K14" t="n">
         <v>9</v>
@@ -1205,18 +1153,14 @@
       <c r="G15" t="n">
         <v>5</v>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H15" t="n">
+        <v>0.7</v>
       </c>
       <c r="I15" t="n">
         <v>166</v>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
+      <c r="J15" t="n">
+        <v>0.33</v>
       </c>
       <c r="K15" t="n">
         <v>4</v>
@@ -1257,18 +1201,14 @@
       <c r="G16" t="n">
         <v>-2</v>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H16" t="n">
+        <v>0.65</v>
       </c>
       <c r="I16" t="n">
         <v>118</v>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>14%</t>
-        </is>
+      <c r="J16" t="n">
+        <v>0.14</v>
       </c>
       <c r="K16" t="n">
         <v>1</v>
@@ -1309,18 +1249,14 @@
       <c r="G17" t="n">
         <v>17</v>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>86%</t>
-        </is>
+      <c r="H17" t="n">
+        <v>0.86</v>
       </c>
       <c r="I17" t="n">
         <v>219</v>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>31%</t>
-        </is>
+      <c r="J17" t="n">
+        <v>0.31</v>
       </c>
       <c r="K17" t="n">
         <v>7</v>
@@ -1361,18 +1297,14 @@
       <c r="G18" t="n">
         <v>2</v>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H18" t="n">
+        <v>0.7</v>
       </c>
       <c r="I18" t="n">
         <v>143</v>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="J18" t="n">
+        <v>0.25</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
@@ -1413,18 +1345,14 @@
       <c r="G19" t="n">
         <v>-9</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>58%</t>
-        </is>
+      <c r="H19" t="n">
+        <v>0.58</v>
       </c>
       <c r="I19" t="n">
         <v>90</v>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>12%</t>
-        </is>
+      <c r="J19" t="n">
+        <v>0.12</v>
       </c>
       <c r="K19" t="n">
         <v>2</v>
@@ -1465,18 +1393,14 @@
       <c r="G20" t="n">
         <v>1</v>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>64%</t>
-        </is>
+      <c r="H20" t="n">
+        <v>0.64</v>
       </c>
       <c r="I20" t="n">
         <v>149</v>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>12%</t>
-        </is>
+      <c r="J20" t="n">
+        <v>0.12</v>
       </c>
       <c r="K20" t="n">
         <v>3</v>
@@ -1517,18 +1441,14 @@
       <c r="G21" t="n">
         <v>1</v>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>85%</t>
-        </is>
+      <c r="H21" t="n">
+        <v>0.85</v>
       </c>
       <c r="I21" t="n">
         <v>154</v>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="J21" t="n">
+        <v>0.27</v>
       </c>
       <c r="K21" t="n">
         <v>6</v>
@@ -1569,18 +1489,14 @@
       <c r="G22" t="n">
         <v>2</v>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>78%</t>
-        </is>
+      <c r="H22" t="n">
+        <v>0.78</v>
       </c>
       <c r="I22" t="n">
         <v>169</v>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>21%</t>
-        </is>
+      <c r="J22" t="n">
+        <v>0.21</v>
       </c>
       <c r="K22" t="n">
         <v>2</v>
@@ -1621,18 +1537,14 @@
       <c r="G23" t="n">
         <v>1</v>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>68%</t>
-        </is>
+      <c r="H23" t="n">
+        <v>0.68</v>
       </c>
       <c r="I23" t="n">
         <v>105</v>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
+      <c r="J23" t="n">
+        <v>0.33</v>
       </c>
       <c r="K23" t="n">
         <v>2</v>
@@ -1673,18 +1585,14 @@
       <c r="G24" t="n">
         <v>-1</v>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>68%</t>
-        </is>
+      <c r="H24" t="n">
+        <v>0.68</v>
       </c>
       <c r="I24" t="n">
         <v>141</v>
       </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>22%</t>
-        </is>
+      <c r="J24" t="n">
+        <v>0.22</v>
       </c>
       <c r="K24" t="n">
         <v>3</v>
@@ -1725,18 +1633,14 @@
       <c r="G25" t="n">
         <v>-9</v>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H25" t="n">
+        <v>0.74</v>
       </c>
       <c r="I25" t="n">
         <v>90</v>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="J25" t="n">
+        <v>0.27</v>
       </c>
       <c r="K25" t="n">
         <v>2</v>
@@ -1777,18 +1681,14 @@
       <c r="G26" t="n">
         <v>4</v>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H26" t="n">
+        <v>0.74</v>
       </c>
       <c r="I26" t="n">
         <v>138</v>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="J26" t="n">
+        <v>0.27</v>
       </c>
       <c r="K26" t="n">
         <v>2</v>
@@ -1829,18 +1729,14 @@
       <c r="G27" t="n">
         <v>-8</v>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H27" t="n">
+        <v>0.65</v>
       </c>
       <c r="I27" t="n">
         <v>94</v>
       </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>24%</t>
-        </is>
+      <c r="J27" t="n">
+        <v>0.24</v>
       </c>
       <c r="K27" t="n">
         <v>2</v>
@@ -1881,18 +1777,14 @@
       <c r="G28" t="n">
         <v>2</v>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H28" t="n">
+        <v>0.65</v>
       </c>
       <c r="I28" t="n">
         <v>173</v>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>23%</t>
-        </is>
+      <c r="J28" t="n">
+        <v>0.23</v>
       </c>
       <c r="K28" t="n">
         <v>5</v>
@@ -1933,18 +1825,14 @@
       <c r="G29" t="n">
         <v>9</v>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H29" t="n">
+        <v>0.74</v>
       </c>
       <c r="I29" t="n">
         <v>160</v>
       </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
+      <c r="J29" t="n">
+        <v>0.33</v>
       </c>
       <c r="K29" t="n">
         <v>1</v>
@@ -1985,18 +1873,14 @@
       <c r="G30" t="n">
         <v>-4</v>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H30" t="n">
+        <v>0.74</v>
       </c>
       <c r="I30" t="n">
         <v>111</v>
       </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>24%</t>
-        </is>
+      <c r="J30" t="n">
+        <v>0.24</v>
       </c>
       <c r="K30" t="n">
         <v>2</v>
@@ -2037,18 +1921,14 @@
       <c r="G31" t="n">
         <v>4</v>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H31" t="n">
+        <v>0.65</v>
       </c>
       <c r="I31" t="n">
         <v>138</v>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>50%</t>
-        </is>
+      <c r="J31" t="n">
+        <v>0.5</v>
       </c>
       <c r="K31" t="n">
         <v>2</v>
@@ -2089,18 +1969,14 @@
       <c r="G32" t="n">
         <v>-2</v>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>90%</t>
-        </is>
+      <c r="H32" t="n">
+        <v>0.9</v>
       </c>
       <c r="I32" t="n">
         <v>113</v>
       </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>29%</t>
-        </is>
+      <c r="J32" t="n">
+        <v>0.29</v>
       </c>
       <c r="K32" t="n">
         <v>1</v>
@@ -2141,18 +2017,14 @@
       <c r="G33" t="n">
         <v>-4</v>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H33" t="n">
+        <v>0.65</v>
       </c>
       <c r="I33" t="n">
         <v>130</v>
       </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>38%</t>
-        </is>
+      <c r="J33" t="n">
+        <v>0.38</v>
       </c>
       <c r="K33" t="n">
         <v>2</v>
@@ -2193,18 +2065,14 @@
       <c r="G34" t="n">
         <v>9</v>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>94%</t>
-        </is>
+      <c r="H34" t="n">
+        <v>0.9399999999999999</v>
       </c>
       <c r="I34" t="n">
         <v>157</v>
       </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="J34" t="n">
+        <v>0.25</v>
       </c>
       <c r="K34" t="n">
         <v>2</v>
@@ -2245,18 +2113,14 @@
       <c r="G35" t="n">
         <v>2</v>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
+      <c r="H35" t="n">
+        <v>0.75</v>
       </c>
       <c r="I35" t="n">
         <v>118</v>
       </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>37%</t>
-        </is>
+      <c r="J35" t="n">
+        <v>0.37</v>
       </c>
       <c r="K35" t="n">
         <v>2</v>
@@ -2297,18 +2161,14 @@
       <c r="G36" t="n">
         <v>8</v>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>67%</t>
-        </is>
+      <c r="H36" t="n">
+        <v>0.67</v>
       </c>
       <c r="I36" t="n">
         <v>126</v>
       </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>29%</t>
-        </is>
+      <c r="J36" t="n">
+        <v>0.29</v>
       </c>
       <c r="K36" t="n">
         <v>1</v>
@@ -2349,18 +2209,14 @@
       <c r="G37" t="n">
         <v>-1</v>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>61%</t>
-        </is>
+      <c r="H37" t="n">
+        <v>0.61</v>
       </c>
       <c r="I37" t="n">
         <v>113</v>
       </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>28%</t>
-        </is>
+      <c r="J37" t="n">
+        <v>0.28</v>
       </c>
       <c r="K37" t="n">
         <v>3</v>
@@ -2401,18 +2257,14 @@
       <c r="G38" t="n">
         <v>-5</v>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>53%</t>
-        </is>
+      <c r="H38" t="n">
+        <v>0.53</v>
       </c>
       <c r="I38" t="n">
         <v>143</v>
       </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>20%</t>
-        </is>
+      <c r="J38" t="n">
+        <v>0.2</v>
       </c>
       <c r="K38" t="n">
         <v>1</v>
@@ -2453,18 +2305,14 @@
       <c r="G39" t="n">
         <v>1</v>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>88%</t>
-        </is>
+      <c r="H39" t="n">
+        <v>0.88</v>
       </c>
       <c r="I39" t="n">
         <v>142</v>
       </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>20%</t>
-        </is>
+      <c r="J39" t="n">
+        <v>0.2</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
@@ -2505,18 +2353,14 @@
       <c r="G40" t="n">
         <v>-8</v>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>56%</t>
-        </is>
+      <c r="H40" t="n">
+        <v>0.5600000000000001</v>
       </c>
       <c r="I40" t="n">
         <v>55</v>
       </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>22%</t>
-        </is>
+      <c r="J40" t="n">
+        <v>0.22</v>
       </c>
       <c r="K40" t="n">
         <v>1</v>
@@ -2557,18 +2401,14 @@
       <c r="G41" t="n">
         <v>-3</v>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H41" t="n">
+        <v>0.65</v>
       </c>
       <c r="I41" t="n">
         <v>139</v>
       </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>36%</t>
-        </is>
+      <c r="J41" t="n">
+        <v>0.36</v>
       </c>
       <c r="K41" t="n">
         <v>3</v>
@@ -2609,18 +2449,14 @@
       <c r="G42" t="n">
         <v>-6</v>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>52%</t>
-        </is>
+      <c r="H42" t="n">
+        <v>0.52</v>
       </c>
       <c r="I42" t="n">
         <v>143</v>
       </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>44%</t>
-        </is>
+      <c r="J42" t="n">
+        <v>0.44</v>
       </c>
       <c r="K42" t="n">
         <v>0</v>
@@ -2661,18 +2497,14 @@
       <c r="G43" t="n">
         <v>-3</v>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>57%</t>
-        </is>
+      <c r="H43" t="n">
+        <v>0.57</v>
       </c>
       <c r="I43" t="n">
         <v>98</v>
       </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
+      <c r="J43" t="n">
+        <v>0.33</v>
       </c>
       <c r="K43" t="n">
         <v>2</v>
@@ -2713,18 +2545,14 @@
       <c r="G44" t="n">
         <v>-4</v>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>59%</t>
-        </is>
+      <c r="H44" t="n">
+        <v>0.59</v>
       </c>
       <c r="I44" t="n">
         <v>78</v>
       </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="J44" t="n">
+        <v>0.25</v>
       </c>
       <c r="K44" t="n">
         <v>0</v>
@@ -2765,18 +2593,14 @@
       <c r="G45" t="n">
         <v>-4</v>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H45" t="n">
+        <v>0.74</v>
       </c>
       <c r="I45" t="n">
         <v>98</v>
       </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>59%</t>
-        </is>
+      <c r="J45" t="n">
+        <v>0.59</v>
       </c>
       <c r="K45" t="n">
         <v>0</v>
@@ -2817,18 +2641,14 @@
       <c r="G46" t="n">
         <v>-5</v>
       </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H46" t="n">
+        <v>0.7</v>
       </c>
       <c r="I46" t="n">
         <v>105</v>
       </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>35%</t>
-        </is>
+      <c r="J46" t="n">
+        <v>0.35</v>
       </c>
       <c r="K46" t="n">
         <v>4</v>
@@ -2869,18 +2689,14 @@
       <c r="G47" t="n">
         <v>-4</v>
       </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H47" t="n">
+        <v>0.65</v>
       </c>
       <c r="I47" t="n">
         <v>112</v>
       </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>18%</t>
-        </is>
+      <c r="J47" t="n">
+        <v>0.18</v>
       </c>
       <c r="K47" t="n">
         <v>2</v>
@@ -2921,18 +2737,14 @@
       <c r="G48" t="n">
         <v>8</v>
       </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>85%</t>
-        </is>
+      <c r="H48" t="n">
+        <v>0.85</v>
       </c>
       <c r="I48" t="n">
         <v>163</v>
       </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J48" t="n">
+        <v>0.26</v>
       </c>
       <c r="K48" t="n">
         <v>2</v>
@@ -2973,18 +2785,14 @@
       <c r="G49" t="n">
         <v>0</v>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H49" t="n">
+        <v>0.65</v>
       </c>
       <c r="I49" t="n">
         <v>127</v>
       </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>23%</t>
-        </is>
+      <c r="J49" t="n">
+        <v>0.23</v>
       </c>
       <c r="K49" t="n">
         <v>1</v>
@@ -3025,18 +2833,14 @@
       <c r="G50" t="n">
         <v>-5</v>
       </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H50" t="n">
+        <v>0.7</v>
       </c>
       <c r="I50" t="n">
         <v>111</v>
       </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>39%</t>
-        </is>
+      <c r="J50" t="n">
+        <v>0.39</v>
       </c>
       <c r="K50" t="n">
         <v>1</v>
@@ -3077,18 +2881,14 @@
       <c r="G51" t="n">
         <v>-1</v>
       </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>80%</t>
-        </is>
+      <c r="H51" t="n">
+        <v>0.8</v>
       </c>
       <c r="I51" t="n">
         <v>118</v>
       </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>13%</t>
-        </is>
+      <c r="J51" t="n">
+        <v>0.13</v>
       </c>
       <c r="K51" t="n">
         <v>1</v>
@@ -3129,18 +2929,14 @@
       <c r="G52" t="n">
         <v>-9</v>
       </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>38%</t>
-        </is>
+      <c r="H52" t="n">
+        <v>0.38</v>
       </c>
       <c r="I52" t="n">
         <v>90</v>
       </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="J52" t="n">
+        <v>0.25</v>
       </c>
       <c r="K52" t="n">
         <v>1</v>
@@ -3181,18 +2977,14 @@
       <c r="G53" t="n">
         <v>-4</v>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>61%</t>
-        </is>
+      <c r="H53" t="n">
+        <v>0.61</v>
       </c>
       <c r="I53" t="n">
         <v>145</v>
       </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>18%</t>
-        </is>
+      <c r="J53" t="n">
+        <v>0.18</v>
       </c>
       <c r="K53" t="n">
         <v>4</v>
@@ -3233,18 +3025,14 @@
       <c r="G54" t="n">
         <v>-5</v>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H54" t="n">
+        <v>0.74</v>
       </c>
       <c r="I54" t="n">
         <v>122</v>
       </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>20%</t>
-        </is>
+      <c r="J54" t="n">
+        <v>0.2</v>
       </c>
       <c r="K54" t="n">
         <v>4</v>
@@ -3285,18 +3073,14 @@
       <c r="G55" t="n">
         <v>1</v>
       </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
+      <c r="H55" t="n">
+        <v>0.75</v>
       </c>
       <c r="I55" t="n">
         <v>161</v>
       </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="J55" t="n">
+        <v>0.27</v>
       </c>
       <c r="K55" t="n">
         <v>7</v>
@@ -3337,18 +3121,14 @@
       <c r="G56" t="n">
         <v>-7</v>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>48%</t>
-        </is>
+      <c r="H56" t="n">
+        <v>0.48</v>
       </c>
       <c r="I56" t="n">
         <v>124</v>
       </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>12%</t>
-        </is>
+      <c r="J56" t="n">
+        <v>0.12</v>
       </c>
       <c r="K56" t="n">
         <v>6</v>
@@ -3389,18 +3169,14 @@
       <c r="G57" t="n">
         <v>-1</v>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>59%</t>
-        </is>
+      <c r="H57" t="n">
+        <v>0.59</v>
       </c>
       <c r="I57" t="n">
         <v>152</v>
       </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>31%</t>
-        </is>
+      <c r="J57" t="n">
+        <v>0.31</v>
       </c>
       <c r="K57" t="n">
         <v>6</v>
@@ -3441,18 +3217,14 @@
       <c r="G58" t="n">
         <v>-6</v>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
+      <c r="H58" t="n">
+        <v>0.62</v>
       </c>
       <c r="I58" t="n">
         <v>99</v>
       </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="J58" t="n">
+        <v>0.27</v>
       </c>
       <c r="K58" t="n">
         <v>0</v>
@@ -3493,18 +3265,14 @@
       <c r="G59" t="n">
         <v>6</v>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>83%</t>
-        </is>
+      <c r="H59" t="n">
+        <v>0.83</v>
       </c>
       <c r="I59" t="n">
         <v>124</v>
       </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>14%</t>
-        </is>
+      <c r="J59" t="n">
+        <v>0.14</v>
       </c>
       <c r="K59" t="n">
         <v>0</v>
@@ -3545,18 +3313,14 @@
       <c r="G60" t="n">
         <v>3</v>
       </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>89%</t>
-        </is>
+      <c r="H60" t="n">
+        <v>0.89</v>
       </c>
       <c r="I60" t="n">
         <v>170</v>
       </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>13%</t>
-        </is>
+      <c r="J60" t="n">
+        <v>0.13</v>
       </c>
       <c r="K60" t="n">
         <v>4</v>
@@ -3597,18 +3361,14 @@
       <c r="G61" t="n">
         <v>9</v>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>94%</t>
-        </is>
+      <c r="H61" t="n">
+        <v>0.9399999999999999</v>
       </c>
       <c r="I61" t="n">
         <v>168</v>
       </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>22%</t>
-        </is>
+      <c r="J61" t="n">
+        <v>0.22</v>
       </c>
       <c r="K61" t="n">
         <v>3</v>
@@ -3649,18 +3409,14 @@
       <c r="G62" t="n">
         <v>3</v>
       </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>83%</t>
-        </is>
+      <c r="H62" t="n">
+        <v>0.83</v>
       </c>
       <c r="I62" t="n">
         <v>149</v>
       </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
+      <c r="J62" t="n">
+        <v>0.3</v>
       </c>
       <c r="K62" t="n">
         <v>5</v>
@@ -3701,18 +3457,14 @@
       <c r="G63" t="n">
         <v>-2</v>
       </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>61%</t>
-        </is>
+      <c r="H63" t="n">
+        <v>0.61</v>
       </c>
       <c r="I63" t="n">
         <v>108</v>
       </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>23%</t>
-        </is>
+      <c r="J63" t="n">
+        <v>0.23</v>
       </c>
       <c r="K63" t="n">
         <v>2</v>
@@ -3753,18 +3505,14 @@
       <c r="G64" t="n">
         <v>-5</v>
       </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>63%</t>
-        </is>
+      <c r="H64" t="n">
+        <v>0.63</v>
       </c>
       <c r="I64" t="n">
         <v>108</v>
       </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>36%</t>
-        </is>
+      <c r="J64" t="n">
+        <v>0.36</v>
       </c>
       <c r="K64" t="n">
         <v>1</v>
@@ -3805,18 +3553,14 @@
       <c r="G65" t="n">
         <v>-9</v>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H65" t="n">
+        <v>0.7</v>
       </c>
       <c r="I65" t="n">
         <v>67</v>
       </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>23%</t>
-        </is>
+      <c r="J65" t="n">
+        <v>0.23</v>
       </c>
       <c r="K65" t="n">
         <v>1</v>
@@ -3857,18 +3601,14 @@
       <c r="G66" t="n">
         <v>-2</v>
       </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>73%</t>
-        </is>
+      <c r="H66" t="n">
+        <v>0.73</v>
       </c>
       <c r="I66" t="n">
         <v>90</v>
       </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>52%</t>
-        </is>
+      <c r="J66" t="n">
+        <v>0.52</v>
       </c>
       <c r="K66" t="n">
         <v>0</v>
@@ -3909,18 +3649,14 @@
       <c r="G67" t="n">
         <v>-7</v>
       </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>52%</t>
-        </is>
+      <c r="H67" t="n">
+        <v>0.52</v>
       </c>
       <c r="I67" t="n">
         <v>76</v>
       </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>38%</t>
-        </is>
+      <c r="J67" t="n">
+        <v>0.38</v>
       </c>
       <c r="K67" t="n">
         <v>1</v>
@@ -3961,18 +3697,14 @@
       <c r="G68" t="n">
         <v>15</v>
       </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>79%</t>
-        </is>
+      <c r="H68" t="n">
+        <v>0.79</v>
       </c>
       <c r="I68" t="n">
         <v>191</v>
       </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>36%</t>
-        </is>
+      <c r="J68" t="n">
+        <v>0.36</v>
       </c>
       <c r="K68" t="n">
         <v>8</v>
@@ -4013,18 +3745,14 @@
       <c r="G69" t="n">
         <v>4</v>
       </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>94%</t>
-        </is>
+      <c r="H69" t="n">
+        <v>0.9399999999999999</v>
       </c>
       <c r="I69" t="n">
         <v>132</v>
       </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>29%</t>
-        </is>
+      <c r="J69" t="n">
+        <v>0.29</v>
       </c>
       <c r="K69" t="n">
         <v>3</v>
@@ -4065,18 +3793,14 @@
       <c r="G70" t="n">
         <v>4</v>
       </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>71%</t>
-        </is>
+      <c r="H70" t="n">
+        <v>0.71</v>
       </c>
       <c r="I70" t="n">
         <v>143</v>
       </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>43%</t>
-        </is>
+      <c r="J70" t="n">
+        <v>0.43</v>
       </c>
       <c r="K70" t="n">
         <v>3</v>
@@ -4117,18 +3841,14 @@
       <c r="G71" t="n">
         <v>-6</v>
       </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>58%</t>
-        </is>
+      <c r="H71" t="n">
+        <v>0.58</v>
       </c>
       <c r="I71" t="n">
         <v>92</v>
       </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>35%</t>
-        </is>
+      <c r="J71" t="n">
+        <v>0.35</v>
       </c>
       <c r="K71" t="n">
         <v>2</v>
@@ -4169,18 +3889,14 @@
       <c r="G72" t="n">
         <v>0</v>
       </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>85%</t>
-        </is>
+      <c r="H72" t="n">
+        <v>0.85</v>
       </c>
       <c r="I72" t="n">
         <v>71</v>
       </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="J72" t="n">
+        <v>0.25</v>
       </c>
       <c r="K72" t="n">
         <v>0</v>
@@ -4221,18 +3937,14 @@
       <c r="G73" t="n">
         <v>-7</v>
       </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>53%</t>
-        </is>
+      <c r="H73" t="n">
+        <v>0.53</v>
       </c>
       <c r="I73" t="n">
         <v>97</v>
       </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="J73" t="n">
+        <v>0.27</v>
       </c>
       <c r="K73" t="n">
         <v>0</v>
@@ -4273,18 +3985,14 @@
       <c r="G74" t="n">
         <v>-6</v>
       </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
+      <c r="H74" t="n">
+        <v>0.62</v>
       </c>
       <c r="I74" t="n">
         <v>79</v>
       </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>22%</t>
-        </is>
+      <c r="J74" t="n">
+        <v>0.22</v>
       </c>
       <c r="K74" t="n">
         <v>1</v>
@@ -4325,18 +4033,14 @@
       <c r="G75" t="n">
         <v>5</v>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>78%</t>
-        </is>
+      <c r="H75" t="n">
+        <v>0.78</v>
       </c>
       <c r="I75" t="n">
         <v>153</v>
       </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J75" t="n">
+        <v>0.26</v>
       </c>
       <c r="K75" t="n">
         <v>1</v>
@@ -4377,18 +4081,14 @@
       <c r="G76" t="n">
         <v>4</v>
       </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>63%</t>
-        </is>
+      <c r="H76" t="n">
+        <v>0.63</v>
       </c>
       <c r="I76" t="n">
         <v>119</v>
       </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>35%</t>
-        </is>
+      <c r="J76" t="n">
+        <v>0.35</v>
       </c>
       <c r="K76" t="n">
         <v>0</v>
@@ -4429,18 +4129,14 @@
       <c r="G77" t="n">
         <v>3</v>
       </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>81%</t>
-        </is>
+      <c r="H77" t="n">
+        <v>0.8100000000000001</v>
       </c>
       <c r="I77" t="n">
         <v>85</v>
       </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>35%</t>
-        </is>
+      <c r="J77" t="n">
+        <v>0.35</v>
       </c>
       <c r="K77" t="n">
         <v>0</v>
@@ -4481,18 +4177,14 @@
       <c r="G78" t="n">
         <v>-4</v>
       </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H78" t="n">
+        <v>0.74</v>
       </c>
       <c r="I78" t="n">
         <v>128</v>
       </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>37%</t>
-        </is>
+      <c r="J78" t="n">
+        <v>0.37</v>
       </c>
       <c r="K78" t="n">
         <v>1</v>
@@ -4533,18 +4225,14 @@
       <c r="G79" t="n">
         <v>-4</v>
       </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>56%</t>
-        </is>
+      <c r="H79" t="n">
+        <v>0.5600000000000001</v>
       </c>
       <c r="I79" t="n">
         <v>124</v>
       </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>43%</t>
-        </is>
+      <c r="J79" t="n">
+        <v>0.43</v>
       </c>
       <c r="K79" t="n">
         <v>0</v>
@@ -4585,18 +4273,14 @@
       <c r="G80" t="n">
         <v>13</v>
       </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>59%</t>
-        </is>
+      <c r="H80" t="n">
+        <v>0.59</v>
       </c>
       <c r="I80" t="n">
         <v>175</v>
       </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>20%</t>
-        </is>
+      <c r="J80" t="n">
+        <v>0.2</v>
       </c>
       <c r="K80" t="n">
         <v>2</v>
@@ -4637,18 +4321,14 @@
       <c r="G81" t="n">
         <v>-1</v>
       </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>78%</t>
-        </is>
+      <c r="H81" t="n">
+        <v>0.78</v>
       </c>
       <c r="I81" t="n">
         <v>136</v>
       </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="J81" t="n">
+        <v>0.27</v>
       </c>
       <c r="K81" t="n">
         <v>2</v>
@@ -4689,18 +4369,14 @@
       <c r="G82" t="n">
         <v>-5</v>
       </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>57%</t>
-        </is>
+      <c r="H82" t="n">
+        <v>0.57</v>
       </c>
       <c r="I82" t="n">
         <v>105</v>
       </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J82" t="n">
+        <v>0.26</v>
       </c>
       <c r="K82" t="n">
         <v>2</v>
@@ -4741,18 +4417,14 @@
       <c r="G83" t="n">
         <v>-5</v>
       </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H83" t="n">
+        <v>0.7</v>
       </c>
       <c r="I83" t="n">
         <v>105</v>
       </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>40%</t>
-        </is>
+      <c r="J83" t="n">
+        <v>0.4</v>
       </c>
       <c r="K83" t="n">
         <v>1</v>
@@ -4793,18 +4465,14 @@
       <c r="G84" t="n">
         <v>0</v>
       </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H84" t="n">
+        <v>0.74</v>
       </c>
       <c r="I84" t="n">
         <v>145</v>
       </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
+      <c r="J84" t="n">
+        <v>0.3</v>
       </c>
       <c r="K84" t="n">
         <v>4</v>
@@ -4845,18 +4513,14 @@
       <c r="G85" t="n">
         <v>0</v>
       </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>63%</t>
-        </is>
+      <c r="H85" t="n">
+        <v>0.63</v>
       </c>
       <c r="I85" t="n">
         <v>153</v>
       </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>38%</t>
-        </is>
+      <c r="J85" t="n">
+        <v>0.38</v>
       </c>
       <c r="K85" t="n">
         <v>3</v>
@@ -4897,18 +4561,14 @@
       <c r="G86" t="n">
         <v>-10</v>
       </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>53%</t>
-        </is>
+      <c r="H86" t="n">
+        <v>0.53</v>
       </c>
       <c r="I86" t="n">
         <v>102</v>
       </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J86" t="n">
+        <v>0.26</v>
       </c>
       <c r="K86" t="n">
         <v>2</v>
@@ -4949,18 +4609,14 @@
       <c r="G87" t="n">
         <v>-7</v>
       </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>59%</t>
-        </is>
+      <c r="H87" t="n">
+        <v>0.59</v>
       </c>
       <c r="I87" t="n">
         <v>107</v>
       </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>34%</t>
-        </is>
+      <c r="J87" t="n">
+        <v>0.34</v>
       </c>
       <c r="K87" t="n">
         <v>2</v>
@@ -5001,18 +4657,14 @@
       <c r="G88" t="n">
         <v>-8</v>
       </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H88" t="n">
+        <v>0.65</v>
       </c>
       <c r="I88" t="n">
         <v>64</v>
       </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>19%</t>
-        </is>
+      <c r="J88" t="n">
+        <v>0.19</v>
       </c>
       <c r="K88" t="n">
         <v>2</v>
@@ -5053,18 +4705,14 @@
       <c r="G89" t="n">
         <v>-1</v>
       </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>60%</t>
-        </is>
+      <c r="H89" t="n">
+        <v>0.6</v>
       </c>
       <c r="I89" t="n">
         <v>89</v>
       </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J89" t="n">
+        <v>0.26</v>
       </c>
       <c r="K89" t="n">
         <v>1</v>
@@ -5105,18 +4753,14 @@
       <c r="G90" t="n">
         <v>4</v>
       </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>81%</t>
-        </is>
+      <c r="H90" t="n">
+        <v>0.8100000000000001</v>
       </c>
       <c r="I90" t="n">
         <v>101</v>
       </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
+      <c r="J90" t="n">
+        <v>0.33</v>
       </c>
       <c r="K90" t="n">
         <v>2</v>
@@ -5157,18 +4801,14 @@
       <c r="G91" t="n">
         <v>7</v>
       </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>76%</t>
-        </is>
+      <c r="H91" t="n">
+        <v>0.76</v>
       </c>
       <c r="I91" t="n">
         <v>125</v>
       </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>39%</t>
-        </is>
+      <c r="J91" t="n">
+        <v>0.39</v>
       </c>
       <c r="K91" t="n">
         <v>1</v>
@@ -5209,18 +4849,14 @@
       <c r="G92" t="n">
         <v>-8</v>
       </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>35%</t>
-        </is>
+      <c r="H92" t="n">
+        <v>0.35</v>
       </c>
       <c r="I92" t="n">
         <v>71</v>
       </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>58%</t>
-        </is>
+      <c r="J92" t="n">
+        <v>0.58</v>
       </c>
       <c r="K92" t="n">
         <v>1</v>
@@ -5261,18 +4897,14 @@
       <c r="G93" t="n">
         <v>2</v>
       </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H93" t="n">
+        <v>0.7</v>
       </c>
       <c r="I93" t="n">
         <v>116</v>
       </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>24%</t>
-        </is>
+      <c r="J93" t="n">
+        <v>0.24</v>
       </c>
       <c r="K93" t="n">
         <v>2</v>
@@ -5313,18 +4945,14 @@
       <c r="G94" t="n">
         <v>-4</v>
       </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>63%</t>
-        </is>
+      <c r="H94" t="n">
+        <v>0.63</v>
       </c>
       <c r="I94" t="n">
         <v>129</v>
       </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J94" t="n">
+        <v>0.26</v>
       </c>
       <c r="K94" t="n">
         <v>2</v>
@@ -5365,18 +4993,14 @@
       <c r="G95" t="n">
         <v>9</v>
       </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
+      <c r="H95" t="n">
+        <v>0.75</v>
       </c>
       <c r="I95" t="n">
         <v>197</v>
       </c>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>29%</t>
-        </is>
+      <c r="J95" t="n">
+        <v>0.29</v>
       </c>
       <c r="K95" t="n">
         <v>0</v>
@@ -5417,18 +5041,14 @@
       <c r="G96" t="n">
         <v>5</v>
       </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>94%</t>
-        </is>
+      <c r="H96" t="n">
+        <v>0.9399999999999999</v>
       </c>
       <c r="I96" t="n">
         <v>121</v>
       </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>38%</t>
-        </is>
+      <c r="J96" t="n">
+        <v>0.38</v>
       </c>
       <c r="K96" t="n">
         <v>1</v>
@@ -5469,18 +5089,14 @@
       <c r="G97" t="n">
         <v>-1</v>
       </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
+      <c r="H97" t="n">
+        <v>0.75</v>
       </c>
       <c r="I97" t="n">
         <v>125</v>
       </c>
-      <c r="J97" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J97" t="n">
+        <v>0.26</v>
       </c>
       <c r="K97" t="n">
         <v>3</v>
@@ -5521,18 +5137,14 @@
       <c r="G98" t="n">
         <v>-2</v>
       </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>68%</t>
-        </is>
+      <c r="H98" t="n">
+        <v>0.68</v>
       </c>
       <c r="I98" t="n">
         <v>136</v>
       </c>
-      <c r="J98" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J98" t="n">
+        <v>0.26</v>
       </c>
       <c r="K98" t="n">
         <v>3</v>
@@ -5573,18 +5185,14 @@
       <c r="G99" t="n">
         <v>5</v>
       </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H99" t="n">
+        <v>0.74</v>
       </c>
       <c r="I99" t="n">
         <v>151</v>
       </c>
-      <c r="J99" t="inlineStr">
-        <is>
-          <t>39%</t>
-        </is>
+      <c r="J99" t="n">
+        <v>0.39</v>
       </c>
       <c r="K99" t="n">
         <v>2</v>
@@ -5625,18 +5233,14 @@
       <c r="G100" t="n">
         <v>7</v>
       </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>82%</t>
-        </is>
+      <c r="H100" t="n">
+        <v>0.82</v>
       </c>
       <c r="I100" t="n">
         <v>152</v>
       </c>
-      <c r="J100" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="J100" t="n">
+        <v>0.27</v>
       </c>
       <c r="K100" t="n">
         <v>3</v>
@@ -5677,18 +5281,14 @@
       <c r="G101" t="n">
         <v>-1</v>
       </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>58%</t>
-        </is>
+      <c r="H101" t="n">
+        <v>0.58</v>
       </c>
       <c r="I101" t="n">
         <v>124</v>
       </c>
-      <c r="J101" t="inlineStr">
-        <is>
-          <t>15%</t>
-        </is>
+      <c r="J101" t="n">
+        <v>0.15</v>
       </c>
       <c r="K101" t="n">
         <v>0</v>
@@ -5729,18 +5329,14 @@
       <c r="G102" t="n">
         <v>2</v>
       </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>91%</t>
-        </is>
+      <c r="H102" t="n">
+        <v>0.91</v>
       </c>
       <c r="I102" t="n">
         <v>107</v>
       </c>
-      <c r="J102" t="inlineStr">
-        <is>
-          <t>29%</t>
-        </is>
+      <c r="J102" t="n">
+        <v>0.29</v>
       </c>
       <c r="K102" t="n">
         <v>3</v>
@@ -5781,18 +5377,14 @@
       <c r="G103" t="n">
         <v>3</v>
       </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t>77%</t>
-        </is>
+      <c r="H103" t="n">
+        <v>0.77</v>
       </c>
       <c r="I103" t="n">
         <v>124</v>
       </c>
-      <c r="J103" t="inlineStr">
-        <is>
-          <t>35%</t>
-        </is>
+      <c r="J103" t="n">
+        <v>0.35</v>
       </c>
       <c r="K103" t="n">
         <v>3</v>
@@ -5833,18 +5425,14 @@
       <c r="G104" t="n">
         <v>5</v>
       </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
+      <c r="H104" t="n">
+        <v>0.75</v>
       </c>
       <c r="I104" t="n">
         <v>137</v>
       </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="J104" t="n">
+        <v>0.25</v>
       </c>
       <c r="K104" t="n">
         <v>4</v>
@@ -5885,18 +5473,14 @@
       <c r="G105" t="n">
         <v>7</v>
       </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H105" t="n">
+        <v>0.7</v>
       </c>
       <c r="I105" t="n">
         <v>172</v>
       </c>
-      <c r="J105" t="inlineStr">
-        <is>
-          <t>31%</t>
-        </is>
+      <c r="J105" t="n">
+        <v>0.31</v>
       </c>
       <c r="K105" t="n">
         <v>4</v>
@@ -5937,18 +5521,14 @@
       <c r="G106" t="n">
         <v>-1</v>
       </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>67%</t>
-        </is>
+      <c r="H106" t="n">
+        <v>0.67</v>
       </c>
       <c r="I106" t="n">
         <v>126</v>
       </c>
-      <c r="J106" t="inlineStr">
-        <is>
-          <t>21%</t>
-        </is>
+      <c r="J106" t="n">
+        <v>0.21</v>
       </c>
       <c r="K106" t="n">
         <v>3</v>
@@ -5989,18 +5569,14 @@
       <c r="G107" t="n">
         <v>5</v>
       </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>71%</t>
-        </is>
+      <c r="H107" t="n">
+        <v>0.71</v>
       </c>
       <c r="I107" t="n">
         <v>169</v>
       </c>
-      <c r="J107" t="inlineStr">
-        <is>
-          <t>29%</t>
-        </is>
+      <c r="J107" t="n">
+        <v>0.29</v>
       </c>
       <c r="K107" t="n">
         <v>1</v>
@@ -6041,18 +5617,14 @@
       <c r="G108" t="n">
         <v>13</v>
       </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>76%</t>
-        </is>
+      <c r="H108" t="n">
+        <v>0.76</v>
       </c>
       <c r="I108" t="n">
         <v>219</v>
       </c>
-      <c r="J108" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J108" t="n">
+        <v>0.26</v>
       </c>
       <c r="K108" t="n">
         <v>6</v>
@@ -6093,18 +5665,14 @@
       <c r="G109" t="n">
         <v>4</v>
       </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>79%</t>
-        </is>
+      <c r="H109" t="n">
+        <v>0.79</v>
       </c>
       <c r="I109" t="n">
         <v>117</v>
       </c>
-      <c r="J109" t="inlineStr">
-        <is>
-          <t>17%</t>
-        </is>
+      <c r="J109" t="n">
+        <v>0.17</v>
       </c>
       <c r="K109" t="n">
         <v>0</v>
@@ -6145,18 +5713,14 @@
       <c r="G110" t="n">
         <v>6</v>
       </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>78%</t>
-        </is>
+      <c r="H110" t="n">
+        <v>0.78</v>
       </c>
       <c r="I110" t="n">
         <v>156</v>
       </c>
-      <c r="J110" t="inlineStr">
-        <is>
-          <t>49%</t>
-        </is>
+      <c r="J110" t="n">
+        <v>0.49</v>
       </c>
       <c r="K110" t="n">
         <v>4</v>
@@ -6197,18 +5761,14 @@
       <c r="G111" t="n">
         <v>-3</v>
       </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
+      <c r="H111" t="n">
+        <v>0.7</v>
       </c>
       <c r="I111" t="n">
         <v>106</v>
       </c>
-      <c r="J111" t="inlineStr">
-        <is>
-          <t>40%</t>
-        </is>
+      <c r="J111" t="n">
+        <v>0.4</v>
       </c>
       <c r="K111" t="n">
         <v>0</v>
@@ -6249,18 +5809,14 @@
       <c r="G112" t="n">
         <v>-5</v>
       </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="H112" t="n">
+        <v>0.74</v>
       </c>
       <c r="I112" t="n">
         <v>136</v>
       </c>
-      <c r="J112" t="inlineStr">
-        <is>
-          <t>35%</t>
-        </is>
+      <c r="J112" t="n">
+        <v>0.35</v>
       </c>
       <c r="K112" t="n">
         <v>0</v>
@@ -6301,18 +5857,14 @@
       <c r="G113" t="n">
         <v>-1</v>
       </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t>64%</t>
-        </is>
+      <c r="H113" t="n">
+        <v>0.64</v>
       </c>
       <c r="I113" t="n">
         <v>111</v>
       </c>
-      <c r="J113" t="inlineStr">
-        <is>
-          <t>36%</t>
-        </is>
+      <c r="J113" t="n">
+        <v>0.36</v>
       </c>
       <c r="K113" t="n">
         <v>1</v>
@@ -6353,18 +5905,14 @@
       <c r="G114" t="n">
         <v>1</v>
       </c>
-      <c r="H114" t="inlineStr">
-        <is>
-          <t>71%</t>
-        </is>
+      <c r="H114" t="n">
+        <v>0.71</v>
       </c>
       <c r="I114" t="n">
         <v>130</v>
       </c>
-      <c r="J114" t="inlineStr">
-        <is>
-          <t>26%</t>
-        </is>
+      <c r="J114" t="n">
+        <v>0.26</v>
       </c>
       <c r="K114" t="n">
         <v>6</v>
@@ -6405,18 +5953,14 @@
       <c r="G115" t="n">
         <v>0</v>
       </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H115" t="n">
+        <v>0.65</v>
       </c>
       <c r="I115" t="n">
         <v>146</v>
       </c>
-      <c r="J115" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="J115" t="n">
+        <v>0.27</v>
       </c>
       <c r="K115" t="n">
         <v>3</v>
@@ -6457,18 +6001,14 @@
       <c r="G116" t="n">
         <v>5</v>
       </c>
-      <c r="H116" t="inlineStr">
-        <is>
-          <t>69%</t>
-        </is>
+      <c r="H116" t="n">
+        <v>0.6899999999999999</v>
       </c>
       <c r="I116" t="n">
         <v>185</v>
       </c>
-      <c r="J116" t="inlineStr">
-        <is>
-          <t>39%</t>
-        </is>
+      <c r="J116" t="n">
+        <v>0.39</v>
       </c>
       <c r="K116" t="n">
         <v>3</v>
@@ -6509,18 +6049,14 @@
       <c r="G117" t="n">
         <v>4</v>
       </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
+      <c r="H117" t="n">
+        <v>0.65</v>
       </c>
       <c r="I117" t="n">
         <v>140</v>
       </c>
-      <c r="J117" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
+      <c r="J117" t="n">
+        <v>0.3</v>
       </c>
       <c r="K117" t="n">
         <v>4</v>
@@ -6561,18 +6097,14 @@
       <c r="G118" t="n">
         <v>8</v>
       </c>
-      <c r="H118" t="inlineStr">
-        <is>
-          <t>86%</t>
-        </is>
+      <c r="H118" t="n">
+        <v>0.86</v>
       </c>
       <c r="I118" t="n">
         <v>134</v>
       </c>
-      <c r="J118" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
+      <c r="J118" t="n">
+        <v>0.33</v>
       </c>
       <c r="K118" t="n">
         <v>2</v>
@@ -6613,18 +6145,14 @@
       <c r="G119" t="n">
         <v>-10</v>
       </c>
-      <c r="H119" t="inlineStr">
-        <is>
-          <t>41%</t>
-        </is>
+      <c r="H119" t="n">
+        <v>0.41</v>
       </c>
       <c r="I119" t="n">
         <v>70</v>
       </c>
-      <c r="J119" t="inlineStr">
-        <is>
-          <t>19%</t>
-        </is>
+      <c r="J119" t="n">
+        <v>0.19</v>
       </c>
       <c r="K119" t="n">
         <v>0</v>
@@ -6665,18 +6193,14 @@
       <c r="G120" t="n">
         <v>11</v>
       </c>
-      <c r="H120" t="inlineStr">
-        <is>
-          <t>85%</t>
-        </is>
+      <c r="H120" t="n">
+        <v>0.85</v>
       </c>
       <c r="I120" t="n">
         <v>181</v>
       </c>
-      <c r="J120" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="J120" t="n">
+        <v>0.25</v>
       </c>
       <c r="K120" t="n">
         <v>3</v>
@@ -6717,18 +6241,14 @@
       <c r="G121" t="n">
         <v>-1</v>
       </c>
-      <c r="H121" t="inlineStr">
-        <is>
-          <t>71%</t>
-        </is>
+      <c r="H121" t="n">
+        <v>0.71</v>
       </c>
       <c r="I121" t="n">
         <v>144</v>
       </c>
-      <c r="J121" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="J121" t="n">
+        <v>0.25</v>
       </c>
       <c r="K121" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
Added URLS to excel
</commit_message>
<xml_diff>
--- a/Player_Stats_Per_Map.xlsx
+++ b/Player_Stats_Per_Map.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N121"/>
+  <dimension ref="A1:O121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,11 @@
           <t>Team</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -552,6 +557,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -600,6 +610,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -648,6 +663,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -696,6 +716,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -744,6 +769,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -792,6 +822,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -840,6 +875,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -888,6 +928,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -936,6 +981,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -984,6 +1034,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1032,6 +1087,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1080,6 +1140,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1128,6 +1193,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1176,6 +1246,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1224,6 +1299,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1272,6 +1352,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1320,6 +1405,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1368,6 +1458,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1416,6 +1511,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1464,6 +1564,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1512,6 +1617,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1560,6 +1670,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1608,6 +1723,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1656,6 +1776,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1704,6 +1829,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1752,6 +1882,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1800,6 +1935,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1848,6 +1988,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1896,6 +2041,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1944,6 +2094,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1992,6 +2147,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2040,6 +2200,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2088,6 +2253,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2136,6 +2306,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2184,6 +2359,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2232,6 +2412,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2280,6 +2465,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2328,6 +2518,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2376,6 +2571,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2424,6 +2624,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2472,6 +2677,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2520,6 +2730,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2568,6 +2783,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2616,6 +2836,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2664,6 +2889,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2712,6 +2942,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2760,6 +2995,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2808,6 +3048,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2856,6 +3101,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2904,6 +3154,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2952,6 +3207,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3000,6 +3260,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3048,6 +3313,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3096,6 +3366,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3144,6 +3419,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3192,6 +3472,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3240,6 +3525,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3288,6 +3578,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3336,6 +3631,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3384,6 +3684,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3432,6 +3737,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3480,6 +3790,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3528,6 +3843,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3576,6 +3896,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3624,6 +3949,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3672,6 +4002,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3720,6 +4055,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3768,6 +4108,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3816,6 +4161,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3864,6 +4214,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3912,6 +4267,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3960,6 +4320,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4008,6 +4373,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4056,6 +4426,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4104,6 +4479,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4152,6 +4532,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4200,6 +4585,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4248,6 +4638,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4296,6 +4691,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4344,6 +4744,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4392,6 +4797,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4440,6 +4850,11 @@
           <t>GE</t>
         </is>
       </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4488,6 +4903,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4536,6 +4956,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4584,6 +5009,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4632,6 +5062,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4680,6 +5115,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4728,6 +5168,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4776,6 +5221,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4824,6 +5274,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4872,6 +5327,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4920,6 +5380,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4968,6 +5433,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5016,6 +5486,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -5064,6 +5539,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5112,6 +5592,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5160,6 +5645,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5208,6 +5698,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5256,6 +5751,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -5304,6 +5804,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -5352,6 +5857,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5400,6 +5910,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -5448,6 +5963,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -5496,6 +6016,11 @@
           <t>GEN</t>
         </is>
       </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -5544,6 +6069,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -5592,6 +6122,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5640,6 +6175,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5688,6 +6228,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -5736,6 +6281,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5784,6 +6334,11 @@
           <t>RRQ</t>
         </is>
       </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296749/gen-g-vs-rex-regum-qeon-champions-tour-2024-pacific-kickoff-decider-c/?game=155171&amp;tab=overview</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -5832,6 +6387,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5880,6 +6440,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5928,6 +6493,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296735/t1-vs-bleed-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5976,6 +6546,11 @@
           <t>BLD</t>
         </is>
       </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296738/bleed-vs-global-esports-champions-tour-2024-pacific-kickoff-elim-a</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -6024,6 +6599,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -6072,6 +6652,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -6120,6 +6705,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296739/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-decider-a</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -6168,6 +6758,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -6216,6 +6811,11 @@
           <t>ZETA</t>
         </is>
       </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296730/zeta-division-vs-global-esports-champions-tour-2024-pacific-kickoff-opening-a</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -6262,6 +6862,11 @@
       <c r="N121" t="inlineStr">
         <is>
           <t>ZETA</t>
+        </is>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>https://www.vlr.gg/296737/t1-vs-zeta-division-champions-tour-2024-pacific-kickoff-winners-a</t>
         </is>
       </c>
     </row>

</xml_diff>